<commit_message>
update file excel untuk latihan power pivot
</commit_message>
<xml_diff>
--- a/Cookie Types.xlsx
+++ b/Cookie Types.xlsx
@@ -1,34 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b09f9559f6a16b6c/Videos/Tutorials/Power Pivot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Downloads\OneDrive-2023-06-21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA73673E-3DD8-4540-82AC-DB0D8015E262}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDDD0EA-2CA9-4D36-A0AC-BC8EA9C4171B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="23070" windowHeight="9735" xr2:uid="{551CB6E8-C087-4EE1-9287-931EDBA32DD8}"/>
+    <workbookView xWindow="16065" yWindow="2700" windowWidth="12555" windowHeight="11505" xr2:uid="{551CB6E8-C087-4EE1-9287-931EDBA32DD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Cookie Types" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -68,8 +58,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="2">
+    <numFmt numFmtId="42" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -117,12 +108,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -146,6 +137,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="32" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -164,6 +156,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="32" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -520,7 +513,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,10 +539,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -557,10 +550,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C3" s="2">
-        <v>0.5</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,10 +561,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="C4" s="2">
-        <v>2.2000000000000002</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -579,10 +572,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="C5" s="2">
-        <v>1.5</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,10 +583,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="C6" s="2">
-        <v>1.25</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -601,16 +594,17 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>6</v>
+        <v>6000</v>
       </c>
       <c r="C7" s="2">
-        <v>2.75</v>
+        <v>2750</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>